<commit_message>
Added BOTRUNNER to run botj notifier and reply
</commit_message>
<xml_diff>
--- a/src/main/java/bot/data.xlsx
+++ b/src/main/java/bot/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kusha\OneDrive\Desktop\oops\src\main\java\bot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1410F7BE-2372-4958-81D9-E0421B3E3765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B86F21-61A9-4147-86CF-03039DF39409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -360,7 +360,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -390,7 +390,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>6304460986</v>
+        <v>5535869992</v>
       </c>
       <c r="C2">
         <v>5625334180</v>

</xml_diff>